<commit_message>
Corrección del guión y esqueleto, eliminación rec
Se eliminó el recurso nuevo ya que tuvimos inconvenientes con el video a
proyectar, por lo tanto se hizo modificación del recurso a uno
aprovechado
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion12/EsqueletoGuion_CN_06_12_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion12/EsqueletoGuion_CN_06_12_CO.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="89">
   <si>
     <t>FICHA</t>
   </si>
@@ -223,9 +223,6 @@
     <t>si</t>
   </si>
   <si>
-    <t>La energía en la naturaleza</t>
-  </si>
-  <si>
     <t>Características de la energía</t>
   </si>
   <si>
@@ -293,13 +290,19 @@
   </si>
   <si>
     <t>Valoración del agua como fuente de energía</t>
+  </si>
+  <si>
+    <t>La evolución histórica de las fuentes de energía</t>
+  </si>
+  <si>
+    <t>CN_06_11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,6 +377,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -878,7 +887,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -946,6 +955,18 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="401">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
@@ -1699,10 +1720,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D23"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1737,51 +1758,51 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="38">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="C2" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="F2" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="38">
+        <v>6</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F3" s="38">
         <v>2</v>
       </c>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
-        <v>6</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="14">
-        <v>4</v>
-      </c>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="14">
@@ -1793,14 +1814,14 @@
       <c r="C4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D4" s="34" t="s">
-        <v>43</v>
+      <c r="D4" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="14">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1813,14 +1834,14 @@
       <c r="C5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>44</v>
+      <c r="D5" s="34" t="s">
+        <v>43</v>
       </c>
       <c r="E5" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F5" s="14">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1834,13 +1855,13 @@
         <v>37</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F6" s="14">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1854,33 +1875,33 @@
         <v>37</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>41</v>
       </c>
       <c r="F7" s="14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="14">
+        <v>6</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="14">
         <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="15">
-        <v>6</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="15">
-        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1894,15 +1915,14 @@
         <v>37</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="15">
-        <v>10</v>
-      </c>
-      <c r="G9" s="7"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
@@ -1915,13 +1935,13 @@
         <v>37</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F10" s="15">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G10" s="7"/>
     </row>
@@ -1936,13 +1956,13 @@
         <v>37</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F11" s="15">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="7"/>
     </row>
@@ -1957,13 +1977,13 @@
         <v>37</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F12" s="15">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G12" s="7"/>
     </row>
@@ -1978,14 +1998,15 @@
         <v>37</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F13" s="15">
-        <v>14</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
@@ -1998,13 +2019,13 @@
         <v>37</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F14" s="15">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2018,13 +2039,13 @@
         <v>37</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F15" s="15">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2038,13 +2059,13 @@
         <v>37</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E16" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F16" s="15">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2058,13 +2079,13 @@
         <v>37</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F17" s="15">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2078,33 +2099,33 @@
         <v>37</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>41</v>
       </c>
       <c r="F18" s="15">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>6</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="15">
         <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="33">
-        <v>6</v>
-      </c>
-      <c r="B19" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="33" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="33">
-        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2118,13 +2139,13 @@
         <v>37</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="33" t="s">
         <v>41</v>
       </c>
       <c r="F20" s="33">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2138,13 +2159,13 @@
         <v>37</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="33" t="s">
         <v>41</v>
       </c>
       <c r="F21" s="33">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -2158,13 +2179,13 @@
         <v>37</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="33" t="s">
         <v>41</v>
       </c>
       <c r="F22" s="33">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2178,12 +2199,32 @@
         <v>37</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>41</v>
       </c>
       <c r="F23" s="33">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="33">
+        <v>6</v>
+      </c>
+      <c r="B24" s="33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="33" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="33">
         <v>24</v>
       </c>
     </row>
@@ -2200,10 +2241,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2223,51 +2264,40 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="13">
-        <v>1</v>
+      <c r="B2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="14">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="14" t="s">
+      <c r="A3" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="14">
-        <v>3</v>
+      <c r="C3" s="32">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B4" s="32" t="s">
         <v>20</v>
       </c>
       <c r="C4" s="32">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="32">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -2287,7 +2317,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2313,10 +2343,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2613,8 +2643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="I99" sqref="I99"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,10 +2823,10 @@
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="13" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -2814,7 +2844,7 @@
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
       <c r="H10" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>19</v>
@@ -2829,7 +2859,7 @@
       </c>
       <c r="C11" s="19"/>
       <c r="D11" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>23</v>
@@ -2848,7 +2878,7 @@
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>24</v>
@@ -2867,7 +2897,7 @@
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>23</v>
@@ -2886,7 +2916,7 @@
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>24</v>
@@ -2905,7 +2935,7 @@
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>23</v>
@@ -2924,7 +2954,7 @@
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>24</v>
@@ -2943,7 +2973,7 @@
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>23</v>
@@ -2962,7 +2992,7 @@
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>24</v>
@@ -2981,7 +3011,7 @@
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>29</v>
@@ -3027,7 +3057,7 @@
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
       <c r="H21" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>20</v>
@@ -3038,7 +3068,7 @@
         <v>37</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C22" s="24" t="s">
         <v>23</v>
@@ -3055,7 +3085,7 @@
         <v>37</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C23" s="24" t="s">
         <v>24</v>
@@ -3072,11 +3102,11 @@
         <v>37</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C24" s="24"/>
       <c r="D24" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E24" s="26" t="s">
         <v>23</v>
@@ -3091,15 +3121,15 @@
         <v>37</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G25" s="26" t="s">
         <v>23</v>
@@ -3112,13 +3142,13 @@
         <v>37</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C26" s="24"/>
       <c r="D26" s="25"/>
       <c r="E26" s="26"/>
       <c r="F26" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G26" s="26" t="s">
         <v>23</v>
@@ -3131,13 +3161,13 @@
         <v>37</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="24"/>
       <c r="D27" s="25"/>
       <c r="E27" s="26"/>
       <c r="F27" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G27" s="26" t="s">
         <v>24</v>
@@ -3150,13 +3180,13 @@
         <v>37</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="25"/>
       <c r="E28" s="26"/>
       <c r="F28" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G28" s="26" t="s">
         <v>23</v>
@@ -3169,13 +3199,13 @@
         <v>37</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" s="24"/>
       <c r="D29" s="25"/>
       <c r="E29" s="26"/>
       <c r="F29" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G29" s="26" t="s">
         <v>26</v>
@@ -3188,13 +3218,13 @@
         <v>37</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C30" s="24"/>
       <c r="D30" s="25"/>
       <c r="E30" s="26"/>
       <c r="F30" s="27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G30" s="26" t="s">
         <v>25</v>
@@ -3211,7 +3241,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C31" s="24"/>
       <c r="D31" s="25" t="s">
@@ -3230,7 +3260,7 @@
         <v>37</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C32" s="24"/>
       <c r="D32" s="25" t="s">
@@ -3249,7 +3279,7 @@
         <v>37</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="24"/>
       <c r="D33" s="25" t="s">
@@ -3268,7 +3298,7 @@
         <v>37</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="25" t="s">
@@ -3287,7 +3317,7 @@
         <v>37</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="25" t="s">
@@ -3306,7 +3336,7 @@
         <v>37</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="25" t="s">
@@ -3325,11 +3355,11 @@
         <v>37</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C37" s="24"/>
       <c r="D37" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E37" s="26" t="s">
         <v>23</v>
@@ -3344,11 +3374,11 @@
         <v>37</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C38" s="24"/>
       <c r="D38" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E38" s="26" t="s">
         <v>26</v>
@@ -3363,15 +3393,15 @@
         <v>37</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C39" s="24"/>
       <c r="D39" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E39" s="26"/>
       <c r="F39" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G39" s="26" t="s">
         <v>23</v>
@@ -3384,15 +3414,15 @@
         <v>37</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C40" s="24"/>
       <c r="D40" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E40" s="26"/>
       <c r="F40" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G40" s="26" t="s">
         <v>24</v>
@@ -3405,15 +3435,15 @@
         <v>37</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C41" s="24"/>
       <c r="D41" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E41" s="26"/>
       <c r="F41" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G41" s="26" t="s">
         <v>23</v>
@@ -3426,11 +3456,11 @@
         <v>37</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C42" s="24"/>
       <c r="D42" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E42" s="26" t="s">
         <v>23</v>
@@ -3445,7 +3475,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C43" s="24"/>
       <c r="D43" s="25" t="s">
@@ -3464,7 +3494,7 @@
         <v>37</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C44" s="24"/>
       <c r="D44" s="25" t="s">
@@ -3472,7 +3502,7 @@
       </c>
       <c r="E44" s="26"/>
       <c r="F44" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G44" s="26" t="s">
         <v>23</v>
@@ -3485,7 +3515,7 @@
         <v>37</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C45" s="24"/>
       <c r="D45" s="25" t="s">
@@ -3493,7 +3523,7 @@
       </c>
       <c r="E45" s="26"/>
       <c r="F45" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G45" s="26" t="s">
         <v>24</v>
@@ -3506,7 +3536,7 @@
         <v>37</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C46" s="24"/>
       <c r="D46" s="25" t="s">
@@ -3514,7 +3544,7 @@
       </c>
       <c r="E46" s="26"/>
       <c r="F46" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G46" s="26" t="s">
         <v>23</v>
@@ -3527,7 +3557,7 @@
         <v>37</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C47" s="24"/>
       <c r="D47" s="25" t="s">
@@ -3535,7 +3565,7 @@
       </c>
       <c r="E47" s="26"/>
       <c r="F47" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G47" s="26" t="s">
         <v>24</v>
@@ -3548,7 +3578,7 @@
         <v>37</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C48" s="24"/>
       <c r="D48" s="25" t="s">
@@ -3556,7 +3586,7 @@
       </c>
       <c r="E48" s="26"/>
       <c r="F48" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G48" s="26" t="s">
         <v>23</v>
@@ -3569,7 +3599,7 @@
         <v>37</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C49" s="24"/>
       <c r="D49" s="25" t="s">
@@ -3577,7 +3607,7 @@
       </c>
       <c r="E49" s="26"/>
       <c r="F49" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G49" s="26" t="s">
         <v>26</v>
@@ -3590,7 +3620,7 @@
         <v>37</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C50" s="24"/>
       <c r="D50" s="25" t="s">
@@ -3598,7 +3628,7 @@
       </c>
       <c r="E50" s="26"/>
       <c r="F50" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G50" s="26" t="s">
         <v>25</v>
@@ -3615,7 +3645,7 @@
         <v>37</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="25" t="s">
@@ -3634,7 +3664,7 @@
         <v>37</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C52" s="24"/>
       <c r="D52" s="25" t="s">
@@ -3657,7 +3687,7 @@
         <v>37</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C53" s="24"/>
       <c r="D53" s="25" t="s">
@@ -3680,7 +3710,7 @@
         <v>37</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C54" s="24"/>
       <c r="D54" s="25" t="s">
@@ -3703,7 +3733,7 @@
         <v>37</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>23</v>
@@ -3720,7 +3750,7 @@
         <v>37</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C56" s="15" t="s">
         <v>24</v>
@@ -3737,7 +3767,7 @@
         <v>37</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>28</v>
@@ -3758,11 +3788,11 @@
         <v>37</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E58" s="15" t="s">
         <v>23</v>
@@ -3777,11 +3807,11 @@
         <v>37</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E59" s="15" t="s">
         <v>24</v>
@@ -3796,11 +3826,11 @@
         <v>37</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E60" s="15"/>
       <c r="F60" s="15" t="s">
@@ -3817,11 +3847,11 @@
         <v>37</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E61" s="15"/>
       <c r="F61" s="15" t="s">
@@ -3838,11 +3868,11 @@
         <v>37</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E62" s="15"/>
       <c r="F62" s="15" t="s">
@@ -3859,11 +3889,11 @@
         <v>37</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E63" s="15"/>
       <c r="F63" s="15" t="s">
@@ -3880,11 +3910,11 @@
         <v>37</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="15" t="s">
@@ -3905,11 +3935,11 @@
         <v>37</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E65" s="15"/>
       <c r="F65" s="15" t="s">
@@ -3930,15 +3960,15 @@
         <v>37</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E66" s="15"/>
       <c r="F66" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G66" s="15" t="s">
         <v>23</v>
@@ -3951,15 +3981,15 @@
         <v>37</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E67" s="15"/>
       <c r="F67" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G67" s="15" t="s">
         <v>24</v>
@@ -3972,15 +4002,15 @@
         <v>37</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E68" s="15"/>
       <c r="F68" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G68" s="15" t="s">
         <v>23</v>
@@ -3993,15 +4023,15 @@
         <v>37</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C69" s="15"/>
       <c r="D69" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E69" s="15"/>
       <c r="F69" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G69" s="15" t="s">
         <v>25</v>
@@ -4018,15 +4048,15 @@
         <v>37</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C70" s="22"/>
       <c r="D70" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E70" s="22"/>
       <c r="F70" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G70" s="28" t="s">
         <v>28</v>
@@ -4043,15 +4073,15 @@
         <v>37</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C71" s="15"/>
       <c r="D71" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E71" s="15"/>
       <c r="F71" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G71" s="15" t="s">
         <v>23</v>
@@ -4064,15 +4094,15 @@
         <v>37</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C72" s="15"/>
       <c r="D72" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E72" s="15"/>
       <c r="F72" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G72" s="15" t="s">
         <v>24</v>
@@ -4085,15 +4115,15 @@
         <v>37</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E73" s="15"/>
       <c r="F73" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G73" s="15" t="s">
         <v>23</v>
@@ -4106,15 +4136,15 @@
         <v>37</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C74" s="15"/>
       <c r="D74" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E74" s="15"/>
       <c r="F74" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G74" s="15" t="s">
         <v>26</v>
@@ -4127,11 +4157,11 @@
         <v>37</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C75" s="15"/>
       <c r="D75" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E75" s="15"/>
       <c r="F75" s="15" t="s">
@@ -4148,11 +4178,11 @@
         <v>37</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C76" s="15"/>
       <c r="D76" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E76" s="15"/>
       <c r="F76" s="15" t="s">
@@ -4173,15 +4203,15 @@
         <v>37</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E77" s="15"/>
       <c r="F77" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G77" s="15" t="s">
         <v>23</v>
@@ -4194,15 +4224,15 @@
         <v>37</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E78" s="15"/>
       <c r="F78" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G78" s="15" t="s">
         <v>24</v>
@@ -4217,11 +4247,11 @@
         <v>37</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E79" s="15" t="s">
         <v>23</v>
@@ -4236,15 +4266,15 @@
         <v>37</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E80" s="15"/>
       <c r="F80" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G80" s="15" t="s">
         <v>23</v>
@@ -4257,15 +4287,15 @@
         <v>37</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C81" s="15"/>
       <c r="D81" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E81" s="15"/>
       <c r="F81" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G81" s="15" t="s">
         <v>24</v>
@@ -4278,15 +4308,15 @@
         <v>37</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C82" s="15"/>
       <c r="D82" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E82" s="15"/>
       <c r="F82" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G82" s="15" t="s">
         <v>23</v>
@@ -4299,15 +4329,15 @@
         <v>37</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C83" s="15"/>
       <c r="D83" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E83" s="15"/>
       <c r="F83" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G83" s="15" t="s">
         <v>25</v>
@@ -4324,15 +4354,15 @@
         <v>37</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C84" s="15"/>
       <c r="D84" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E84" s="15"/>
       <c r="F84" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G84" s="15" t="s">
         <v>23</v>
@@ -4345,15 +4375,15 @@
         <v>37</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C85" s="15"/>
       <c r="D85" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E85" s="15"/>
       <c r="F85" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G85" s="15" t="s">
         <v>24</v>
@@ -4366,15 +4396,15 @@
         <v>37</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C86" s="15"/>
       <c r="D86" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E86" s="15"/>
       <c r="F86" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G86" s="15" t="s">
         <v>23</v>
@@ -4387,15 +4417,15 @@
         <v>37</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C87" s="15"/>
       <c r="D87" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E87" s="15"/>
       <c r="F87" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G87" s="15" t="s">
         <v>28</v>
@@ -4412,15 +4442,15 @@
         <v>37</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C88" s="15"/>
       <c r="D88" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E88" s="15"/>
       <c r="F88" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G88" s="15" t="s">
         <v>28</v>
@@ -4437,11 +4467,11 @@
         <v>37</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C89" s="15"/>
       <c r="D89" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E89" s="15" t="s">
         <v>23</v>
@@ -4456,11 +4486,11 @@
         <v>37</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C90" s="15"/>
       <c r="D90" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E90" s="15" t="s">
         <v>28</v>
@@ -4479,11 +4509,11 @@
         <v>37</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C91" s="15"/>
       <c r="D91" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E91" s="15" t="s">
         <v>25</v>
@@ -4592,7 +4622,7 @@
       <c r="F96" s="29"/>
       <c r="G96" s="29"/>
       <c r="H96" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I96" s="29" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Correcciones solicitadas por María del Pilar
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion12/EsqueletoGuion_CN_06_12_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion12/EsqueletoGuion_CN_06_12_CO.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mpgarcia\Desktop\CienciasNaturales\fuentes\contenidos\grado06\guion12\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="60" windowWidth="18765" windowHeight="9195" tabRatio="729" activeTab="4"/>
   </bookViews>
@@ -21,7 +16,7 @@
   <definedNames>
     <definedName name="OLE_LINK28" localSheetId="4">'CUADERNO DE ESTUDIO'!$H$54</definedName>
   </definedNames>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="90">
   <si>
     <t>FICHA</t>
   </si>
@@ -301,6 +296,9 @@
   </si>
   <si>
     <t>CN_06_11</t>
+  </si>
+  <si>
+    <t>Qué es la electricidad</t>
   </si>
 </sst>
 </file>
@@ -1644,7 +1642,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2648,8 +2646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3279,26 +3277,24 @@
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>67</v>
-      </c>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
       <c r="C33" s="24"/>
       <c r="D33" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E33" s="26" t="s">
+      <c r="E33" s="26"/>
+      <c r="F33" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G33" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="21" t="s">
         <v>37</v>
       </c>
@@ -3309,11 +3305,13 @@
       <c r="D34" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E34" s="26" t="s">
+      <c r="E34" s="26"/>
+      <c r="F34" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
     </row>
@@ -3328,11 +3326,13 @@
       <c r="D35" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E35" s="26" t="s">
+      <c r="E35" s="26"/>
+      <c r="F35" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G35" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
     </row>
@@ -3347,11 +3347,13 @@
       <c r="D36" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="26" t="s">
+      <c r="E36" s="26"/>
+      <c r="F36" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G36" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
     </row>

</xml_diff>

<commit_message>
Revisión de palabras claves, corrección de esquele
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion12/EsqueletoGuion_CN_06_12_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion12/EsqueletoGuion_CN_06_12_CO.xlsx
@@ -16,7 +16,7 @@
   <definedNames>
     <definedName name="OLE_LINK28" localSheetId="4">'CUADERNO DE ESTUDIO'!$H$54</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" iterateCount="2" iterateDelta="10"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="100">
   <si>
     <t>FICHA</t>
   </si>
@@ -154,27 +154,15 @@
     <t>Refuerza tu aprendizaje: ¿Qué es la energía?</t>
   </si>
   <si>
-    <t>CN_06_12</t>
-  </si>
-  <si>
-    <t>La energía potencial y cinética</t>
-  </si>
-  <si>
     <t>La energía nuclear</t>
   </si>
   <si>
-    <t>Tipos de energía</t>
-  </si>
-  <si>
     <t>Define los tipos de energía</t>
   </si>
   <si>
     <t>La energía solar</t>
   </si>
   <si>
-    <t>Energía eólica: molino</t>
-  </si>
-  <si>
     <t>La energía geotérmica</t>
   </si>
   <si>
@@ -184,21 +172,6 @@
     <t>Fuentes y tipos de energía</t>
   </si>
   <si>
-    <t>Identificación tipos de energía</t>
-  </si>
-  <si>
-    <t>Reconocimiento de las propiedades de la energía</t>
-  </si>
-  <si>
-    <t>Comparación de las fuentes de energía</t>
-  </si>
-  <si>
-    <t>valoración del agua como fuente de energía</t>
-  </si>
-  <si>
-    <t>Realización de un plan de ahorro energético</t>
-  </si>
-  <si>
     <t>La energía eléctrica</t>
   </si>
   <si>
@@ -214,12 +187,6 @@
     <t>¿Qué sabes sobre energía nuclear?</t>
   </si>
   <si>
-    <t>Las fuentes de energía</t>
-  </si>
-  <si>
-    <t>Comprende las fuentes de energía</t>
-  </si>
-  <si>
     <t>si</t>
   </si>
   <si>
@@ -229,9 +196,6 @@
     <t xml:space="preserve">Características de la Energía </t>
   </si>
   <si>
-    <t>¿Qué es la energía?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tipos de energía </t>
   </si>
   <si>
@@ -289,16 +253,82 @@
     <t xml:space="preserve">Consolidación </t>
   </si>
   <si>
-    <t>Valoración del agua como fuente de energía</t>
-  </si>
-  <si>
     <t>La evolución histórica de las fuentes de energía</t>
   </si>
   <si>
-    <t>CN_06_11</t>
-  </si>
-  <si>
     <t>Qué es la electricidad</t>
+  </si>
+  <si>
+    <t>4º ESO</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>Las nuevas fuentes de energía</t>
+  </si>
+  <si>
+    <t>TC_10_07</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>La energía</t>
+  </si>
+  <si>
+    <t>MN_3C_19</t>
+  </si>
+  <si>
+    <t>2° ESO</t>
+  </si>
+  <si>
+    <t>La energía cinética y la potencial</t>
+  </si>
+  <si>
+    <t>CN_08_06</t>
+  </si>
+  <si>
+    <t>La energía: tipos y origen</t>
+  </si>
+  <si>
+    <t>La electricidad</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: La energía eléctrica</t>
+  </si>
+  <si>
+    <t>CN_08_07</t>
+  </si>
+  <si>
+    <t>3° ESO</t>
+  </si>
+  <si>
+    <t>TC_09_14</t>
+  </si>
+  <si>
+    <t>Comprende las principales fuentes de energía</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Competencias: identificación de los tipos de energía</t>
+  </si>
+  <si>
+    <t>Competencias: reconocimiento de las propiedades de la energía</t>
+  </si>
+  <si>
+    <t>Competencias: comparación de las fuentes de energía renovables</t>
+  </si>
+  <si>
+    <t>Competencias: valoración del agua como fuente de energía</t>
+  </si>
+  <si>
+    <t>Competencias: realización de un plan para el ahorro energético</t>
+  </si>
+  <si>
+    <t>Refuerza tu aprendizaje: Las fuentes de energía</t>
   </si>
 </sst>
 </file>
@@ -890,7 +920,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -958,12 +988,6 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1653,7 +1677,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1726,7 +1750,7 @@
   <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1762,42 +1786,42 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38">
-        <v>6</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="E2" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="37">
+      <c r="A2" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="35">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38">
-        <v>6</v>
-      </c>
-      <c r="B3" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="F3" s="38">
+      <c r="A3" s="13">
+        <v>5</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="36">
         <v>2</v>
       </c>
       <c r="G3"/>
@@ -1808,40 +1832,40 @@
       <c r="L3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="14">
-        <v>6</v>
+      <c r="A4" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="F4" s="14">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="14">
-        <v>6</v>
+      <c r="A5" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="F5" s="14">
         <v>5</v>
@@ -1849,79 +1873,79 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F6" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <v>6</v>
+      <c r="A7" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="F7" s="14">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="14">
-        <v>6</v>
+      <c r="A8" s="14" t="s">
+        <v>83</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>41</v>
+        <v>89</v>
       </c>
       <c r="F8" s="14">
         <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
-        <v>6</v>
+      <c r="A9" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="F9" s="15">
         <v>9</v>
@@ -1929,19 +1953,19 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F10" s="15">
         <v>10</v>
@@ -1949,20 +1973,20 @@
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
-        <v>6</v>
+      <c r="A11" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="F11" s="15">
         <v>11</v>
@@ -1970,20 +1994,20 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
-        <v>6</v>
+      <c r="A12" s="15" t="s">
+        <v>83</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="F12" s="15">
         <v>12</v>
@@ -1992,19 +2016,19 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F13" s="15">
         <v>13</v>
@@ -2012,20 +2036,20 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="15">
-        <v>6</v>
+      <c r="A14" s="15" t="s">
+        <v>90</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="F14" s="15">
         <v>14</v>
@@ -2033,19 +2057,19 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F15" s="15">
         <v>15</v>
@@ -2053,19 +2077,19 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F16" s="15">
         <v>16</v>
@@ -2073,19 +2097,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F17" s="15">
         <v>17</v>
@@ -2093,39 +2117,39 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F18" s="15">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="15">
-        <v>6</v>
+      <c r="A19" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F19" s="15">
         <v>19</v>
@@ -2133,19 +2157,19 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B20" s="33" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D20" s="33" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="E20" s="33" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F20" s="33">
         <v>20</v>
@@ -2153,19 +2177,19 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" s="33" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D21" s="33" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="E21" s="33" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F21" s="33">
         <v>21</v>
@@ -2173,19 +2197,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B22" s="33" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="E22" s="33" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F22" s="33">
         <v>22</v>
@@ -2193,19 +2217,19 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F23" s="33">
         <v>23</v>
@@ -2213,19 +2237,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="F24" s="33">
         <v>24</v>
@@ -2247,7 +2271,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2269,7 +2293,7 @@
     </row>
     <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>20</v>
@@ -2319,8 +2343,8 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2346,10 +2370,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2379,7 +2403,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
@@ -2390,7 +2414,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -2401,7 +2425,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -2412,7 +2436,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -2423,7 +2447,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -2434,7 +2458,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -2445,7 +2469,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -2456,7 +2480,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -2467,7 +2491,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -2478,7 +2502,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
@@ -2489,7 +2513,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
@@ -2500,7 +2524,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
@@ -2511,7 +2535,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
@@ -2522,7 +2546,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
@@ -2533,7 +2557,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
@@ -2544,7 +2568,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
@@ -2555,7 +2579,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
@@ -2566,7 +2590,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
@@ -2577,7 +2601,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
@@ -2588,7 +2612,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
@@ -2599,7 +2623,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
         <v>19</v>
@@ -2646,8 +2670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C43" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="K90" sqref="K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2730,7 +2754,7 @@
       <c r="A4" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="18" t="s">
@@ -2747,7 +2771,7 @@
       <c r="A5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="18" t="s">
@@ -2764,10 +2788,10 @@
       <c r="A6" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="18"/>
@@ -2781,10 +2805,10 @@
       <c r="A7" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="19" t="s">
+      <c r="B7" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="18"/>
@@ -2798,10 +2822,10 @@
       <c r="A8" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="19" t="s">
+      <c r="B8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="18"/>
@@ -2815,10 +2839,10 @@
       <c r="A9" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="19" t="s">
+      <c r="B9" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="18" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="18"/>
@@ -2826,7 +2850,7 @@
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="13" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>19</v>
@@ -2836,10 +2860,10 @@
       <c r="A10" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="19" t="s">
+      <c r="B10" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="18" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="18"/>
@@ -2847,7 +2871,7 @@
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
       <c r="H10" s="13" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>19</v>
@@ -2857,12 +2881,12 @@
       <c r="A11" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="19"/>
+      <c r="B11" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="18"/>
       <c r="D11" s="18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>23</v>
@@ -2881,7 +2905,7 @@
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>24</v>
@@ -2900,7 +2924,7 @@
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>23</v>
@@ -2919,7 +2943,7 @@
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>24</v>
@@ -2938,7 +2962,7 @@
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>23</v>
@@ -2957,7 +2981,7 @@
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>24</v>
@@ -2976,7 +3000,7 @@
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>23</v>
@@ -2995,7 +3019,7 @@
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>24</v>
@@ -3014,7 +3038,7 @@
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="18" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>29</v>
@@ -3060,7 +3084,7 @@
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
       <c r="H21" s="13" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>20</v>
@@ -3071,9 +3095,9 @@
         <v>37</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="25"/>
@@ -3088,9 +3112,9 @@
         <v>37</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="21" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="25"/>
@@ -3105,11 +3129,11 @@
         <v>37</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="24"/>
+        <v>55</v>
+      </c>
+      <c r="C24" s="21"/>
       <c r="D24" s="25" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E24" s="26" t="s">
         <v>23</v>
@@ -3124,15 +3148,15 @@
         <v>37</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="25" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="27" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="G25" s="26" t="s">
         <v>23</v>
@@ -3145,13 +3169,13 @@
         <v>37</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C26" s="24"/>
       <c r="D26" s="25"/>
       <c r="E26" s="26"/>
       <c r="F26" s="27" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="G26" s="26" t="s">
         <v>23</v>
@@ -3164,13 +3188,13 @@
         <v>37</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C27" s="24"/>
       <c r="D27" s="25"/>
       <c r="E27" s="26"/>
       <c r="F27" s="27" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="G27" s="26" t="s">
         <v>24</v>
@@ -3183,13 +3207,13 @@
         <v>37</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="25"/>
       <c r="E28" s="26"/>
       <c r="F28" s="27" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G28" s="26" t="s">
         <v>23</v>
@@ -3202,13 +3226,13 @@
         <v>37</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C29" s="24"/>
       <c r="D29" s="25"/>
       <c r="E29" s="26"/>
       <c r="F29" s="27" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G29" s="26" t="s">
         <v>26</v>
@@ -3221,19 +3245,19 @@
         <v>37</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C30" s="24"/>
       <c r="D30" s="25"/>
       <c r="E30" s="26"/>
       <c r="F30" s="27" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="G30" s="26" t="s">
         <v>25</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>42</v>
+        <v>84</v>
       </c>
       <c r="I30" s="14" t="s">
         <v>19</v>
@@ -3244,11 +3268,11 @@
         <v>37</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C31" s="24"/>
       <c r="D31" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E31" s="26" t="s">
         <v>23</v>
@@ -3263,11 +3287,11 @@
         <v>37</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C32" s="24"/>
       <c r="D32" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E32" s="26" t="s">
         <v>24</v>
@@ -3278,15 +3302,19 @@
       <c r="I32" s="14"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="21"/>
-      <c r="B33" s="21"/>
+      <c r="A33" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="21" t="s">
+        <v>55</v>
+      </c>
       <c r="C33" s="24"/>
       <c r="D33" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E33" s="26"/>
       <c r="F33" s="27" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G33" s="27" t="s">
         <v>23</v>
@@ -3299,15 +3327,15 @@
         <v>37</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E34" s="26"/>
       <c r="F34" s="27" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G34" s="26" t="s">
         <v>24</v>
@@ -3320,15 +3348,15 @@
         <v>37</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E35" s="26"/>
       <c r="F35" s="27" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G35" s="26" t="s">
         <v>26</v>
@@ -3341,15 +3369,15 @@
         <v>37</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="25" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E36" s="26"/>
       <c r="F36" s="27" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="G36" s="26" t="s">
         <v>23</v>
@@ -3362,11 +3390,11 @@
         <v>37</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C37" s="24"/>
       <c r="D37" s="25" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E37" s="26" t="s">
         <v>23</v>
@@ -3381,11 +3409,11 @@
         <v>37</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C38" s="24"/>
       <c r="D38" s="25" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E38" s="26" t="s">
         <v>26</v>
@@ -3400,15 +3428,15 @@
         <v>37</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C39" s="24"/>
       <c r="D39" s="25" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E39" s="26"/>
       <c r="F39" s="26" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="G39" s="26" t="s">
         <v>23</v>
@@ -3421,15 +3449,15 @@
         <v>37</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C40" s="24"/>
       <c r="D40" s="25" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E40" s="26"/>
       <c r="F40" s="26" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="G40" s="26" t="s">
         <v>24</v>
@@ -3442,15 +3470,15 @@
         <v>37</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C41" s="24"/>
       <c r="D41" s="25" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="E41" s="26"/>
       <c r="F41" s="26" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="G41" s="26" t="s">
         <v>23</v>
@@ -3463,11 +3491,11 @@
         <v>37</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C42" s="24"/>
       <c r="D42" s="25" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="E42" s="26" t="s">
         <v>23</v>
@@ -3482,11 +3510,11 @@
         <v>37</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C43" s="24"/>
       <c r="D43" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E43" s="26" t="s">
         <v>23</v>
@@ -3501,15 +3529,15 @@
         <v>37</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C44" s="24"/>
       <c r="D44" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E44" s="26"/>
       <c r="F44" s="26" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="G44" s="26" t="s">
         <v>23</v>
@@ -3522,15 +3550,15 @@
         <v>37</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C45" s="24"/>
       <c r="D45" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E45" s="26"/>
       <c r="F45" s="26" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="G45" s="26" t="s">
         <v>24</v>
@@ -3543,15 +3571,15 @@
         <v>37</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C46" s="24"/>
       <c r="D46" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E46" s="26"/>
       <c r="F46" s="26" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="G46" s="26" t="s">
         <v>23</v>
@@ -3564,15 +3592,15 @@
         <v>37</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C47" s="24"/>
       <c r="D47" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E47" s="26"/>
       <c r="F47" s="26" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="G47" s="26" t="s">
         <v>24</v>
@@ -3585,15 +3613,15 @@
         <v>37</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C48" s="24"/>
       <c r="D48" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E48" s="26"/>
       <c r="F48" s="26" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="G48" s="26" t="s">
         <v>23</v>
@@ -3606,15 +3634,15 @@
         <v>37</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C49" s="24"/>
       <c r="D49" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E49" s="26"/>
       <c r="F49" s="26" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="G49" s="26" t="s">
         <v>26</v>
@@ -3627,21 +3655,21 @@
         <v>37</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C50" s="24"/>
       <c r="D50" s="25" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E50" s="26"/>
       <c r="F50" s="26" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="G50" s="26" t="s">
         <v>25</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="I50" s="14" t="s">
         <v>19</v>
@@ -3652,7 +3680,7 @@
         <v>37</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="25" t="s">
@@ -3671,7 +3699,7 @@
         <v>37</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C52" s="24"/>
       <c r="D52" s="25" t="s">
@@ -3683,7 +3711,7 @@
       <c r="F52" s="26"/>
       <c r="G52" s="26"/>
       <c r="H52" s="14" t="s">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="I52" s="14" t="s">
         <v>19</v>
@@ -3694,7 +3722,7 @@
         <v>37</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C53" s="24"/>
       <c r="D53" s="25" t="s">
@@ -3706,7 +3734,7 @@
       <c r="F53" s="26"/>
       <c r="G53" s="26"/>
       <c r="H53" s="14" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="I53" s="14" t="s">
         <v>19</v>
@@ -3717,7 +3745,7 @@
         <v>37</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C54" s="24"/>
       <c r="D54" s="25" t="s">
@@ -3729,7 +3757,7 @@
       <c r="F54" s="26"/>
       <c r="G54" s="26"/>
       <c r="H54" s="14" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="I54" s="14" t="s">
         <v>19</v>
@@ -3740,7 +3768,7 @@
         <v>37</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>23</v>
@@ -3757,7 +3785,7 @@
         <v>37</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C56" s="15" t="s">
         <v>24</v>
@@ -3774,7 +3802,7 @@
         <v>37</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>28</v>
@@ -3784,7 +3812,7 @@
       <c r="F57" s="15"/>
       <c r="G57" s="15"/>
       <c r="H57" s="15" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="I57" s="15" t="s">
         <v>19</v>
@@ -3795,11 +3823,11 @@
         <v>37</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E58" s="15" t="s">
         <v>23</v>
@@ -3814,11 +3842,11 @@
         <v>37</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E59" s="15" t="s">
         <v>24</v>
@@ -3833,15 +3861,15 @@
         <v>37</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E60" s="15"/>
       <c r="F60" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G60" s="15" t="s">
         <v>23</v>
@@ -3854,15 +3882,15 @@
         <v>37</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E61" s="15"/>
       <c r="F61" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G61" s="15" t="s">
         <v>24</v>
@@ -3875,15 +3903,15 @@
         <v>37</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E62" s="15"/>
       <c r="F62" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G62" s="15" t="s">
         <v>23</v>
@@ -3896,15 +3924,15 @@
         <v>37</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E63" s="15"/>
       <c r="F63" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G63" s="15" t="s">
         <v>29</v>
@@ -3917,21 +3945,21 @@
         <v>37</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G64" s="15" t="s">
         <v>25</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="I64" s="15" t="s">
         <v>19</v>
@@ -3942,21 +3970,21 @@
         <v>37</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E65" s="15"/>
       <c r="F65" s="15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G65" s="15" t="s">
         <v>28</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="I65" s="15" t="s">
         <v>19</v>
@@ -3967,15 +3995,15 @@
         <v>37</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E66" s="15"/>
       <c r="F66" s="15" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G66" s="15" t="s">
         <v>23</v>
@@ -3988,15 +4016,15 @@
         <v>37</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E67" s="15"/>
       <c r="F67" s="15" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G67" s="15" t="s">
         <v>24</v>
@@ -4009,15 +4037,15 @@
         <v>37</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E68" s="15"/>
       <c r="F68" s="15" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G68" s="15" t="s">
         <v>23</v>
@@ -4030,21 +4058,21 @@
         <v>37</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C69" s="15"/>
       <c r="D69" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E69" s="15"/>
       <c r="F69" s="15" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G69" s="15" t="s">
         <v>25</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="I69" s="15" t="s">
         <v>19</v>
@@ -4055,21 +4083,21 @@
         <v>37</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C70" s="22"/>
       <c r="D70" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E70" s="22"/>
       <c r="F70" s="15" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="G70" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="H70" s="22" t="s">
-        <v>59</v>
+      <c r="H70" s="15" t="s">
+        <v>50</v>
       </c>
       <c r="I70" s="28" t="s">
         <v>19</v>
@@ -4080,15 +4108,15 @@
         <v>37</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C71" s="15"/>
       <c r="D71" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E71" s="15"/>
       <c r="F71" s="15" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G71" s="15" t="s">
         <v>23</v>
@@ -4101,15 +4129,15 @@
         <v>37</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C72" s="15"/>
       <c r="D72" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E72" s="15"/>
       <c r="F72" s="15" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G72" s="15" t="s">
         <v>24</v>
@@ -4122,15 +4150,15 @@
         <v>37</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E73" s="15"/>
       <c r="F73" s="15" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G73" s="15" t="s">
         <v>23</v>
@@ -4143,15 +4171,15 @@
         <v>37</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C74" s="15"/>
       <c r="D74" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E74" s="15"/>
       <c r="F74" s="15" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="G74" s="15" t="s">
         <v>26</v>
@@ -4164,15 +4192,15 @@
         <v>37</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C75" s="15"/>
       <c r="D75" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E75" s="15"/>
       <c r="F75" s="15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G75" s="15" t="s">
         <v>23</v>
@@ -4185,21 +4213,21 @@
         <v>37</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C76" s="15"/>
       <c r="D76" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E76" s="15"/>
       <c r="F76" s="15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G76" s="15" t="s">
         <v>25</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="I76" s="15" t="s">
         <v>19</v>
@@ -4210,15 +4238,15 @@
         <v>37</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E77" s="15"/>
       <c r="F77" s="15" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="G77" s="15" t="s">
         <v>23</v>
@@ -4231,15 +4259,15 @@
         <v>37</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="15" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E78" s="15"/>
       <c r="F78" s="15" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="G78" s="15" t="s">
         <v>24</v>
@@ -4254,11 +4282,11 @@
         <v>37</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E79" s="15" t="s">
         <v>23</v>
@@ -4273,15 +4301,15 @@
         <v>37</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E80" s="15"/>
       <c r="F80" s="15" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="G80" s="15" t="s">
         <v>23</v>
@@ -4294,15 +4322,15 @@
         <v>37</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C81" s="15"/>
       <c r="D81" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E81" s="15"/>
       <c r="F81" s="15" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="G81" s="15" t="s">
         <v>24</v>
@@ -4315,15 +4343,15 @@
         <v>37</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C82" s="15"/>
       <c r="D82" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E82" s="15"/>
       <c r="F82" s="15" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="G82" s="15" t="s">
         <v>23</v>
@@ -4336,21 +4364,21 @@
         <v>37</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C83" s="15"/>
       <c r="D83" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E83" s="15"/>
       <c r="F83" s="15" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="G83" s="15" t="s">
         <v>25</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I83" s="15" t="s">
         <v>19</v>
@@ -4361,15 +4389,15 @@
         <v>37</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C84" s="15"/>
       <c r="D84" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E84" s="15"/>
       <c r="F84" s="15" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G84" s="15" t="s">
         <v>23</v>
@@ -4382,15 +4410,15 @@
         <v>37</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C85" s="15"/>
       <c r="D85" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E85" s="15"/>
       <c r="F85" s="15" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G85" s="15" t="s">
         <v>24</v>
@@ -4403,15 +4431,15 @@
         <v>37</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C86" s="15"/>
       <c r="D86" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E86" s="15"/>
       <c r="F86" s="15" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G86" s="15" t="s">
         <v>23</v>
@@ -4424,21 +4452,21 @@
         <v>37</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C87" s="15"/>
       <c r="D87" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E87" s="15"/>
       <c r="F87" s="15" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G87" s="15" t="s">
         <v>28</v>
       </c>
       <c r="H87" s="15" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="I87" s="15" t="s">
         <v>19</v>
@@ -4449,21 +4477,21 @@
         <v>37</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C88" s="15"/>
       <c r="D88" s="15" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E88" s="15"/>
       <c r="F88" s="15" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="G88" s="15" t="s">
         <v>28</v>
       </c>
       <c r="H88" s="15" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
       <c r="I88" s="15" t="s">
         <v>19</v>
@@ -4474,11 +4502,11 @@
         <v>37</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C89" s="15"/>
       <c r="D89" s="15" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E89" s="15" t="s">
         <v>23</v>
@@ -4493,11 +4521,11 @@
         <v>37</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C90" s="15"/>
       <c r="D90" s="15" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E90" s="15" t="s">
         <v>28</v>
@@ -4505,7 +4533,7 @@
       <c r="F90" s="15"/>
       <c r="G90" s="15"/>
       <c r="H90" s="15" t="s">
-        <v>61</v>
+        <v>99</v>
       </c>
       <c r="I90" s="15" t="s">
         <v>19</v>
@@ -4516,11 +4544,11 @@
         <v>37</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C91" s="15"/>
       <c r="D91" s="15" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E91" s="15" t="s">
         <v>25</v>
@@ -4528,7 +4556,7 @@
       <c r="F91" s="15"/>
       <c r="G91" s="15"/>
       <c r="H91" s="15" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I91" s="15" t="s">
         <v>19</v>
@@ -4565,8 +4593,8 @@
       <c r="E93" s="29"/>
       <c r="F93" s="29"/>
       <c r="G93" s="29"/>
-      <c r="H93" s="29" t="s">
-        <v>51</v>
+      <c r="H93" s="16" t="s">
+        <v>94</v>
       </c>
       <c r="I93" s="29" t="s">
         <v>19</v>
@@ -4586,8 +4614,8 @@
       <c r="E94" s="29"/>
       <c r="F94" s="29"/>
       <c r="G94" s="29"/>
-      <c r="H94" s="29" t="s">
-        <v>52</v>
+      <c r="H94" s="16" t="s">
+        <v>95</v>
       </c>
       <c r="I94" s="29" t="s">
         <v>19</v>
@@ -4607,8 +4635,8 @@
       <c r="E95" s="29"/>
       <c r="F95" s="29"/>
       <c r="G95" s="29"/>
-      <c r="H95" s="29" t="s">
-        <v>53</v>
+      <c r="H95" s="16" t="s">
+        <v>96</v>
       </c>
       <c r="I95" s="29" t="s">
         <v>19</v>
@@ -4628,8 +4656,8 @@
       <c r="E96" s="29"/>
       <c r="F96" s="29"/>
       <c r="G96" s="29"/>
-      <c r="H96" s="29" t="s">
-        <v>86</v>
+      <c r="H96" s="16" t="s">
+        <v>97</v>
       </c>
       <c r="I96" s="29" t="s">
         <v>19</v>
@@ -4649,8 +4677,8 @@
       <c r="E97" s="29"/>
       <c r="F97" s="29"/>
       <c r="G97" s="29"/>
-      <c r="H97" s="29" t="s">
-        <v>55</v>
+      <c r="H97" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="I97" s="29" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
CN0612: Ajuste de esqueleto, manuscrito y creación de archivo de seguimiento ProdDigital
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion12/EsqueletoGuion_CN_06_12_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion12/EsqueletoGuion_CN_06_12_CO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Documents\Aula Planeta Colombia\Repositorios\CienciasNaturales\fuentes\contenidos\grado06\guion12\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="18765" windowHeight="9195" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="18765" windowHeight="9198" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="99">
   <si>
     <t>FICHA</t>
   </si>
@@ -125,9 +130,6 @@
   </si>
   <si>
     <t>CN</t>
-  </si>
-  <si>
-    <t>Introducción al movimiento</t>
   </si>
   <si>
     <t>Consolidación</t>
@@ -1666,7 +1668,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1680,45 +1682,45 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1726,7 +1728,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -1753,19 +1755,19 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.1328125" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1785,41 +1787,41 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>78</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>79</v>
       </c>
       <c r="F2" s="35">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="13">
         <v>5</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>81</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>82</v>
       </c>
       <c r="F3" s="36">
         <v>2</v>
@@ -1831,425 +1833,425 @@
       <c r="K3"/>
       <c r="L3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D4" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>84</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>85</v>
       </c>
       <c r="F4" s="14">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F5" s="14">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" s="14">
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="D6" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="F6" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="14">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C8" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="E8" s="14" t="s">
         <v>88</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>89</v>
       </c>
       <c r="F8" s="14">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F9" s="15">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" s="15">
         <v>5</v>
       </c>
       <c r="B10" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="D10" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="15" t="s">
         <v>81</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>82</v>
       </c>
       <c r="F10" s="15">
         <v>10</v>
       </c>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F11" s="15">
         <v>11</v>
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F12" s="15">
         <v>12</v>
       </c>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" s="15">
         <v>5</v>
       </c>
       <c r="B13" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C13" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="D13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="15" t="s">
         <v>81</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>82</v>
       </c>
       <c r="F13" s="15">
         <v>13</v>
       </c>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>90</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C14" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>91</v>
       </c>
       <c r="F14" s="15">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" s="15">
         <v>5</v>
       </c>
       <c r="B15" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C15" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="D15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>81</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>82</v>
       </c>
       <c r="F15" s="15">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" s="15">
         <v>5</v>
       </c>
       <c r="B16" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="D16" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>81</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>82</v>
       </c>
       <c r="F16" s="15">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="15">
         <v>5</v>
       </c>
       <c r="B17" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>81</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>82</v>
       </c>
       <c r="F17" s="15">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="15">
         <v>5</v>
       </c>
       <c r="B18" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="D18" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="15" t="s">
         <v>81</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>82</v>
       </c>
       <c r="F18" s="15">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="D19" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="15" t="s">
         <v>81</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>82</v>
       </c>
       <c r="F19" s="15">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="33">
         <v>5</v>
       </c>
       <c r="B20" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C20" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="33" t="s">
+      <c r="D20" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="E20" s="33" t="s">
         <v>81</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>82</v>
       </c>
       <c r="F20" s="33">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="33">
         <v>5</v>
       </c>
       <c r="B21" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="33" t="s">
+      <c r="D21" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="33" t="s">
         <v>81</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>95</v>
-      </c>
-      <c r="E21" s="33" t="s">
-        <v>82</v>
       </c>
       <c r="F21" s="33">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="33">
         <v>5</v>
       </c>
       <c r="B22" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="D22" s="33" t="s">
+        <v>95</v>
+      </c>
+      <c r="E22" s="33" t="s">
         <v>81</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>96</v>
-      </c>
-      <c r="E22" s="33" t="s">
-        <v>82</v>
       </c>
       <c r="F22" s="33">
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="33">
         <v>5</v>
       </c>
       <c r="B23" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="D23" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" s="33" t="s">
         <v>81</v>
-      </c>
-      <c r="D23" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="E23" s="33" t="s">
-        <v>82</v>
       </c>
       <c r="F23" s="33">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="33">
         <v>5</v>
       </c>
       <c r="B24" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="D24" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="33" t="s">
         <v>81</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" s="33" t="s">
-        <v>82</v>
       </c>
       <c r="F24" s="33">
         <v>24</v>
@@ -2271,16 +2273,16 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -2291,9 +2293,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>20</v>
@@ -2302,9 +2304,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="32" t="s">
         <v>20</v>
@@ -2313,7 +2315,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="32" t="s">
         <v>22</v>
       </c>
@@ -2324,7 +2326,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
@@ -2344,17 +2346,17 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B25"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2365,271 +2367,271 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="13">
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="13">
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="14">
         <v>3</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="14">
         <v>4</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="14">
         <v>5</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="14">
         <v>6</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="14">
         <v>7</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="14">
         <v>8</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="15">
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="15">
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="15">
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="15">
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="15">
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="15">
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="15">
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="15">
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="15">
         <v>17</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="15">
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="15">
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="16">
         <v>20</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="16">
         <v>21</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="16">
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="16">
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="16">
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="31">
         <v>25</v>
       </c>
@@ -2640,7 +2642,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="31">
         <v>26</v>
       </c>
@@ -2670,24 +2672,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="K90" sqref="K90"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="61.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="46.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.59765625" customWidth="1"/>
+    <col min="2" max="2" width="43.86328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="61.265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.86328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="46.1328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -2716,12 +2718,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="18" t="s">
         <v>23</v>
@@ -2733,12 +2735,12 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="18" t="s">
         <v>24</v>
@@ -2750,12 +2752,12 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>23</v>
@@ -2767,12 +2769,12 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>24</v>
@@ -2784,12 +2786,12 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>23</v>
@@ -2801,12 +2803,12 @@
       <c r="H6" s="13"/>
       <c r="I6" s="18"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="18" t="s">
         <v>24</v>
@@ -2818,12 +2820,12 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>26</v>
@@ -2835,12 +2837,12 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>25</v>
@@ -2850,18 +2852,18 @@
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>28</v>
@@ -2871,22 +2873,22 @@
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
       <c r="H10" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>23</v>
@@ -2896,16 +2898,16 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>24</v>
@@ -2915,16 +2917,16 @@
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>23</v>
@@ -2934,16 +2936,16 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="19"/>
       <c r="D14" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>24</v>
@@ -2953,16 +2955,16 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>23</v>
@@ -2972,16 +2974,16 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="19"/>
       <c r="D16" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>24</v>
@@ -2991,16 +2993,16 @@
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>23</v>
@@ -3010,16 +3012,16 @@
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>24</v>
@@ -3029,16 +3031,16 @@
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>29</v>
@@ -3048,16 +3050,16 @@
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="19"/>
       <c r="D20" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>23</v>
@@ -3067,16 +3069,16 @@
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>28</v>
@@ -3084,18 +3086,18 @@
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
       <c r="H21" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>23</v>
@@ -3107,12 +3109,12 @@
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>24</v>
@@ -3124,16 +3126,16 @@
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="21"/>
       <c r="D24" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E24" s="26" t="s">
         <v>23</v>
@@ -3143,20 +3145,20 @@
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C25" s="24"/>
       <c r="D25" s="25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G25" s="26" t="s">
         <v>23</v>
@@ -3164,18 +3166,18 @@
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" s="24"/>
       <c r="D26" s="25"/>
       <c r="E26" s="26"/>
       <c r="F26" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G26" s="26" t="s">
         <v>23</v>
@@ -3183,18 +3185,18 @@
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" s="24"/>
       <c r="D27" s="25"/>
       <c r="E27" s="26"/>
       <c r="F27" s="27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G27" s="26" t="s">
         <v>24</v>
@@ -3202,18 +3204,18 @@
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="24"/>
       <c r="D28" s="25"/>
       <c r="E28" s="26"/>
       <c r="F28" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G28" s="26" t="s">
         <v>23</v>
@@ -3221,18 +3223,18 @@
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="24"/>
       <c r="D29" s="25"/>
       <c r="E29" s="26"/>
       <c r="F29" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G29" s="26" t="s">
         <v>26</v>
@@ -3240,39 +3242,39 @@
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" s="24"/>
       <c r="D30" s="25"/>
       <c r="E30" s="26"/>
       <c r="F30" s="27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G30" s="26" t="s">
         <v>25</v>
       </c>
       <c r="H30" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I30" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="24"/>
       <c r="D31" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E31" s="26" t="s">
         <v>23</v>
@@ -3282,16 +3284,16 @@
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" s="24"/>
       <c r="D32" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E32" s="26" t="s">
         <v>24</v>
@@ -3301,20 +3303,20 @@
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C33" s="24"/>
       <c r="D33" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E33" s="26"/>
       <c r="F33" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G33" s="27" t="s">
         <v>23</v>
@@ -3322,20 +3324,20 @@
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A34" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C34" s="24"/>
       <c r="D34" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E34" s="26"/>
       <c r="F34" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G34" s="26" t="s">
         <v>24</v>
@@ -3343,20 +3345,20 @@
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" s="24"/>
       <c r="D35" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E35" s="26"/>
       <c r="F35" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G35" s="26" t="s">
         <v>26</v>
@@ -3364,20 +3366,20 @@
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" s="24"/>
       <c r="D36" s="25" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E36" s="26"/>
       <c r="F36" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G36" s="26" t="s">
         <v>23</v>
@@ -3385,16 +3387,16 @@
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C37" s="24"/>
       <c r="D37" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E37" s="26" t="s">
         <v>23</v>
@@ -3404,16 +3406,16 @@
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C38" s="24"/>
       <c r="D38" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E38" s="26" t="s">
         <v>26</v>
@@ -3423,20 +3425,20 @@
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C39" s="24"/>
       <c r="D39" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E39" s="26"/>
       <c r="F39" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G39" s="26" t="s">
         <v>23</v>
@@ -3444,20 +3446,20 @@
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" s="24"/>
       <c r="D40" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E40" s="26"/>
       <c r="F40" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G40" s="26" t="s">
         <v>24</v>
@@ -3465,20 +3467,20 @@
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B41" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C41" s="24"/>
       <c r="D41" s="25" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E41" s="26"/>
       <c r="F41" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G41" s="26" t="s">
         <v>23</v>
@@ -3486,16 +3488,16 @@
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C42" s="24"/>
       <c r="D42" s="25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E42" s="26" t="s">
         <v>23</v>
@@ -3505,16 +3507,16 @@
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B43" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="24"/>
       <c r="D43" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E43" s="26" t="s">
         <v>23</v>
@@ -3524,20 +3526,20 @@
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B44" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C44" s="24"/>
       <c r="D44" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E44" s="26"/>
       <c r="F44" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G44" s="26" t="s">
         <v>23</v>
@@ -3545,20 +3547,20 @@
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" s="24"/>
       <c r="D45" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E45" s="26"/>
       <c r="F45" s="26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G45" s="26" t="s">
         <v>24</v>
@@ -3566,20 +3568,20 @@
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="24"/>
       <c r="D46" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E46" s="26"/>
       <c r="F46" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G46" s="26" t="s">
         <v>23</v>
@@ -3587,20 +3589,20 @@
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B47" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C47" s="24"/>
       <c r="D47" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E47" s="26"/>
       <c r="F47" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G47" s="26" t="s">
         <v>24</v>
@@ -3608,20 +3610,20 @@
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B48" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="24"/>
       <c r="D48" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E48" s="26"/>
       <c r="F48" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G48" s="26" t="s">
         <v>23</v>
@@ -3629,20 +3631,20 @@
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B49" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" s="24"/>
       <c r="D49" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E49" s="26"/>
       <c r="F49" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G49" s="26" t="s">
         <v>26</v>
@@ -3650,41 +3652,41 @@
       <c r="H49" s="14"/>
       <c r="I49" s="14"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B50" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C50" s="24"/>
       <c r="D50" s="25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E50" s="26"/>
       <c r="F50" s="26" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G50" s="26" t="s">
         <v>25</v>
       </c>
       <c r="H50" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I50" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B51" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" s="24"/>
       <c r="D51" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E51" s="26" t="s">
         <v>23</v>
@@ -3694,16 +3696,16 @@
       <c r="H51" s="14"/>
       <c r="I51" s="14"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B52" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" s="24"/>
       <c r="D52" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E52" s="26" t="s">
         <v>25</v>
@@ -3711,22 +3713,22 @@
       <c r="F52" s="26"/>
       <c r="G52" s="26"/>
       <c r="H52" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I52" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B53" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C53" s="24"/>
       <c r="D53" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E53" s="26" t="s">
         <v>28</v>
@@ -3734,22 +3736,22 @@
       <c r="F53" s="26"/>
       <c r="G53" s="26"/>
       <c r="H53" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I53" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C54" s="24"/>
       <c r="D54" s="25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E54" s="26" t="s">
         <v>28</v>
@@ -3757,18 +3759,18 @@
       <c r="F54" s="26"/>
       <c r="G54" s="26"/>
       <c r="H54" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I54" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="15" t="s">
         <v>23</v>
@@ -3780,12 +3782,12 @@
       <c r="H55" s="15"/>
       <c r="I55" s="15"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C56" s="15" t="s">
         <v>24</v>
@@ -3797,12 +3799,12 @@
       <c r="H56" s="15"/>
       <c r="I56" s="15"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B57" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>28</v>
@@ -3812,22 +3814,22 @@
       <c r="F57" s="15"/>
       <c r="G57" s="15"/>
       <c r="H57" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I57" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B58" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E58" s="15" t="s">
         <v>23</v>
@@ -3837,16 +3839,16 @@
       <c r="H58" s="15"/>
       <c r="I58" s="15"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E59" s="15" t="s">
         <v>24</v>
@@ -3856,20 +3858,20 @@
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E60" s="15"/>
       <c r="F60" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G60" s="15" t="s">
         <v>23</v>
@@ -3877,20 +3879,20 @@
       <c r="H60" s="15"/>
       <c r="I60" s="15"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E61" s="15"/>
       <c r="F61" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G61" s="15" t="s">
         <v>24</v>
@@ -3898,20 +3900,20 @@
       <c r="H61" s="15"/>
       <c r="I61" s="15"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E62" s="15"/>
       <c r="F62" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G62" s="15" t="s">
         <v>23</v>
@@ -3919,20 +3921,20 @@
       <c r="H62" s="15"/>
       <c r="I62" s="15"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B63" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E63" s="15"/>
       <c r="F63" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G63" s="15" t="s">
         <v>29</v>
@@ -3940,70 +3942,70 @@
       <c r="H63" s="15"/>
       <c r="I63" s="15"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B64" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C64" s="15"/>
       <c r="D64" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G64" s="15" t="s">
         <v>25</v>
       </c>
       <c r="H64" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I64" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65" s="15"/>
       <c r="D65" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E65" s="15"/>
       <c r="F65" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G65" s="15" t="s">
         <v>28</v>
       </c>
       <c r="H65" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I65" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E66" s="15"/>
       <c r="F66" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G66" s="15" t="s">
         <v>23</v>
@@ -4011,20 +4013,20 @@
       <c r="H66" s="15"/>
       <c r="I66" s="15"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E67" s="15"/>
       <c r="F67" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G67" s="15" t="s">
         <v>24</v>
@@ -4032,20 +4034,20 @@
       <c r="H67" s="15"/>
       <c r="I67" s="15"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E68" s="15"/>
       <c r="F68" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G68" s="15" t="s">
         <v>23</v>
@@ -4053,70 +4055,70 @@
       <c r="H68" s="15"/>
       <c r="I68" s="15"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C69" s="15"/>
       <c r="D69" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E69" s="15"/>
       <c r="F69" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G69" s="15" t="s">
         <v>25</v>
       </c>
       <c r="H69" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I69" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C70" s="22"/>
       <c r="D70" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E70" s="22"/>
       <c r="F70" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G70" s="28" t="s">
         <v>28</v>
       </c>
       <c r="H70" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I70" s="28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C71" s="15"/>
       <c r="D71" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E71" s="15"/>
       <c r="F71" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G71" s="15" t="s">
         <v>23</v>
@@ -4124,20 +4126,20 @@
       <c r="H71" s="15"/>
       <c r="I71" s="15"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B72" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C72" s="15"/>
       <c r="D72" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E72" s="15"/>
       <c r="F72" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G72" s="15" t="s">
         <v>24</v>
@@ -4145,20 +4147,20 @@
       <c r="H72" s="15"/>
       <c r="I72" s="15"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E73" s="15"/>
       <c r="F73" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G73" s="15" t="s">
         <v>23</v>
@@ -4166,20 +4168,20 @@
       <c r="H73" s="15"/>
       <c r="I73" s="15"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C74" s="15"/>
       <c r="D74" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E74" s="15"/>
       <c r="F74" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G74" s="15" t="s">
         <v>26</v>
@@ -4187,20 +4189,20 @@
       <c r="H74" s="15"/>
       <c r="I74" s="15"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C75" s="15"/>
       <c r="D75" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E75" s="15"/>
       <c r="F75" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G75" s="15" t="s">
         <v>23</v>
@@ -4208,45 +4210,45 @@
       <c r="H75" s="15"/>
       <c r="I75" s="15"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C76" s="15"/>
       <c r="D76" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E76" s="15"/>
       <c r="F76" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G76" s="15" t="s">
         <v>25</v>
       </c>
       <c r="H76" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I76" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A77" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B77" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E77" s="15"/>
       <c r="F77" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G77" s="15" t="s">
         <v>23</v>
@@ -4254,20 +4256,20 @@
       <c r="H77" s="15"/>
       <c r="I77" s="15"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B78" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E78" s="15"/>
       <c r="F78" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G78" s="15" t="s">
         <v>24</v>
@@ -4277,16 +4279,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E79" s="15" t="s">
         <v>23</v>
@@ -4296,20 +4298,20 @@
       <c r="H79" s="15"/>
       <c r="I79" s="15"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E80" s="15"/>
       <c r="F80" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G80" s="15" t="s">
         <v>23</v>
@@ -4317,20 +4319,20 @@
       <c r="H80" s="15"/>
       <c r="I80" s="15"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B81" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C81" s="15"/>
       <c r="D81" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E81" s="15"/>
       <c r="F81" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G81" s="15" t="s">
         <v>24</v>
@@ -4338,20 +4340,20 @@
       <c r="H81" s="15"/>
       <c r="I81" s="15"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B82" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C82" s="15"/>
       <c r="D82" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E82" s="15"/>
       <c r="F82" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G82" s="15" t="s">
         <v>23</v>
@@ -4359,45 +4361,45 @@
       <c r="H82" s="15"/>
       <c r="I82" s="15"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B83" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C83" s="15"/>
       <c r="D83" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E83" s="15"/>
       <c r="F83" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G83" s="15" t="s">
         <v>25</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I83" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C84" s="15"/>
       <c r="D84" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E84" s="15"/>
       <c r="F84" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G84" s="15" t="s">
         <v>23</v>
@@ -4405,20 +4407,20 @@
       <c r="H84" s="15"/>
       <c r="I84" s="15"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C85" s="15"/>
       <c r="D85" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E85" s="15"/>
       <c r="F85" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G85" s="15" t="s">
         <v>24</v>
@@ -4426,20 +4428,20 @@
       <c r="H85" s="15"/>
       <c r="I85" s="15"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C86" s="15"/>
       <c r="D86" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E86" s="15"/>
       <c r="F86" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G86" s="15" t="s">
         <v>23</v>
@@ -4447,66 +4449,66 @@
       <c r="H86" s="15"/>
       <c r="I86" s="15"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C87" s="15"/>
       <c r="D87" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E87" s="15"/>
       <c r="F87" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G87" s="15" t="s">
         <v>28</v>
       </c>
       <c r="H87" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I87" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C88" s="15"/>
       <c r="D88" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E88" s="15"/>
       <c r="F88" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G88" s="15" t="s">
         <v>28</v>
       </c>
       <c r="H88" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I88" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C89" s="15"/>
       <c r="D89" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E89" s="15" t="s">
         <v>23</v>
@@ -4516,16 +4518,16 @@
       <c r="H89" s="15"/>
       <c r="I89" s="15"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C90" s="15"/>
       <c r="D90" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E90" s="15" t="s">
         <v>28</v>
@@ -4533,22 +4535,22 @@
       <c r="F90" s="15"/>
       <c r="G90" s="15"/>
       <c r="H90" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I90" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C91" s="15"/>
       <c r="D91" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E91" s="15" t="s">
         <v>25</v>
@@ -4556,18 +4558,18 @@
       <c r="F91" s="15"/>
       <c r="G91" s="15"/>
       <c r="H91" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I91" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B92" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C92" s="29" t="s">
         <v>23</v>
@@ -4579,12 +4581,12 @@
       <c r="H92" s="29"/>
       <c r="I92" s="29"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B93" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C93" s="29" t="s">
         <v>28</v>
@@ -4594,18 +4596,18 @@
       <c r="F93" s="29"/>
       <c r="G93" s="29"/>
       <c r="H93" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I93" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B94" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C94" s="29" t="s">
         <v>28</v>
@@ -4615,18 +4617,18 @@
       <c r="F94" s="29"/>
       <c r="G94" s="29"/>
       <c r="H94" s="16" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I94" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B95" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C95" s="29" t="s">
         <v>28</v>
@@ -4636,18 +4638,18 @@
       <c r="F95" s="29"/>
       <c r="G95" s="29"/>
       <c r="H95" s="16" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I95" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B96" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C96" s="29" t="s">
         <v>28</v>
@@ -4657,18 +4659,18 @@
       <c r="F96" s="29"/>
       <c r="G96" s="29"/>
       <c r="H96" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I96" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B97" s="29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C97" s="29" t="s">
         <v>28</v>
@@ -4678,15 +4680,15 @@
       <c r="F97" s="29"/>
       <c r="G97" s="29"/>
       <c r="H97" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I97" s="29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B98" s="30" t="s">
         <v>27</v>
@@ -4703,9 +4705,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B99" s="30" t="s">
         <v>27</v>

</xml_diff>